<commit_message>
Excel con las corridas
</commit_message>
<xml_diff>
--- a/corridas-escenario1.xlsx
+++ b/corridas-escenario1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liza\Desktop\TPSimulacion\TPI-Simulacion-Showcase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larad\Facultad\4to Año\Simulacion\TPI\TPI-Simulacion-Showcase-main (5)\TPI-Simulacion-Showcase-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF41793B-2C76-4BC8-B328-CB6F1B082662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C034E67F-C88D-4249-B050-78C726BE3D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tiempo" sheetId="2" r:id="rId1"/>
@@ -64,7 +64,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +75,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -109,8 +117,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -392,622 +400,1228 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF08E78B-342C-4777-9FFB-6358C0659432}">
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="2" customWidth="1"/>
-    <col min="2" max="2" width="50.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="50.28515625" customWidth="1"/>
     <col min="3" max="3" width="46.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
         <f>ROW(A1)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="B2">
+        <v>83.478260869565403</v>
+      </c>
+      <c r="C2">
+        <v>3.13333333333332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
         <f t="shared" ref="A3:A66" si="0">ROW(A2)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="B3">
+        <v>83.478260869565403</v>
+      </c>
+      <c r="C3">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="B4">
+        <v>82.758620689655402</v>
+      </c>
+      <c r="C4">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="B5">
+        <v>82.758620689655402</v>
+      </c>
+      <c r="C5">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="B6">
+        <v>82.758620689655402</v>
+      </c>
+      <c r="C6">
+        <v>3.0333333333333199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="B7">
+        <v>82.0512820512822</v>
+      </c>
+      <c r="C7">
+        <v>3.1666666666666501</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="B8">
+        <v>84.955752212389598</v>
+      </c>
+      <c r="C8">
+        <v>3.0999999999999899</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="B9">
+        <v>81.355932203389997</v>
+      </c>
+      <c r="C9">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="B10">
+        <v>80.000000000000199</v>
+      </c>
+      <c r="C10">
+        <v>3.2999999999999901</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="B11">
+        <v>79.75</v>
+      </c>
+      <c r="C11">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="B12">
+        <v>83.478260869565403</v>
+      </c>
+      <c r="C12">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="B13">
+        <v>82.758620689655402</v>
+      </c>
+      <c r="C13">
+        <v>3.2333333333333201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="B14">
+        <v>79.75</v>
+      </c>
+      <c r="C14">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="B15">
+        <v>82.758620689655402</v>
+      </c>
+      <c r="C15">
+        <v>3.2666666666666502</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="B16">
+        <v>84.210526315789707</v>
+      </c>
+      <c r="C16">
+        <v>3.13333333333332</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="B17">
+        <v>79.75</v>
+      </c>
+      <c r="C17">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="B18">
+        <v>82.758620689655402</v>
+      </c>
+      <c r="C18">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="B19">
+        <v>81.355932203389997</v>
+      </c>
+      <c r="C19">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="B20">
+        <v>83.478260869565403</v>
+      </c>
+      <c r="C20">
+        <v>3.2333333333333201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="B21">
+        <v>80.672268907563193</v>
+      </c>
+      <c r="C21">
+        <v>3.2666666666666502</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="B22">
+        <v>80.672268907563193</v>
+      </c>
+      <c r="C22">
+        <v>3.2333333333333201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="B23">
+        <v>83.478260869565403</v>
+      </c>
+      <c r="C23">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="B24">
+        <v>79.75</v>
+      </c>
+      <c r="C24">
+        <v>3.2666666666666502</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="B25">
+        <v>84.210526315789707</v>
+      </c>
+      <c r="C25">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="B26">
+        <v>79.75</v>
+      </c>
+      <c r="C26">
+        <v>3.2999999999999901</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="B27">
+        <v>84.210526315789707</v>
+      </c>
+      <c r="C27">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="B28">
+        <v>80.000000000000199</v>
+      </c>
+      <c r="C28">
+        <v>3.2333333333333201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="B29">
+        <v>82.0512820512822</v>
+      </c>
+      <c r="C29">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="B30">
+        <v>80.000000000000199</v>
+      </c>
+      <c r="C30">
+        <v>3.2333333333333201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="B31">
+        <v>83.478260869565403</v>
+      </c>
+      <c r="C31">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="B32">
+        <v>85.714285714285893</v>
+      </c>
+      <c r="C32">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="B33">
+        <v>82.758620689655402</v>
+      </c>
+      <c r="C33">
+        <v>3.13333333333332</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="B34">
+        <v>84.955752212389598</v>
+      </c>
+      <c r="C34">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="B35">
+        <v>83.478260869565403</v>
+      </c>
+      <c r="C35">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+      <c r="B36">
+        <v>85.714285714285893</v>
+      </c>
+      <c r="C36">
+        <v>3.0999999999999899</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+      <c r="B37">
+        <v>82.0512820512822</v>
+      </c>
+      <c r="C37">
+        <v>3.13333333333332</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
+      <c r="B38">
+        <v>80.000000000000199</v>
+      </c>
+      <c r="C38">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
+      <c r="B39">
+        <v>80.000000000000199</v>
+      </c>
+      <c r="C39">
+        <v>3.2333333333333201</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+      <c r="B40">
+        <v>82.0512820512822</v>
+      </c>
+      <c r="C40">
+        <v>3.2333333333333201</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+      <c r="B41">
+        <v>82.758620689655402</v>
+      </c>
+      <c r="C41">
+        <v>3.2333333333333201</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+      <c r="B42">
+        <v>82.0512820512822</v>
+      </c>
+      <c r="C42">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+      <c r="B43">
+        <v>80.000000000000199</v>
+      </c>
+      <c r="C43">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
+      <c r="B44">
+        <v>82.0512820512822</v>
+      </c>
+      <c r="C44">
+        <v>3.2333333333333201</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+      <c r="B45">
+        <v>80.000000000000199</v>
+      </c>
+      <c r="C45">
+        <v>3.2666666666666502</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+      <c r="B46">
+        <v>83.478260869565403</v>
+      </c>
+      <c r="C46">
+        <v>3.06666666666665</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+      <c r="B47">
+        <v>82.758620689655402</v>
+      </c>
+      <c r="C47">
+        <v>3.2333333333333201</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
+      <c r="B48">
+        <v>80.672268907563193</v>
+      </c>
+      <c r="C48">
+        <v>3.2666666666666502</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
+      <c r="B49">
+        <v>82.0512820512822</v>
+      </c>
+      <c r="C49">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
+      <c r="B50">
+        <v>84.210526315789707</v>
+      </c>
+      <c r="C50">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
+      <c r="B51">
+        <v>83.478260869565403</v>
+      </c>
+      <c r="C51">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
+      <c r="B52">
+        <v>84.955752212389598</v>
+      </c>
+      <c r="C52">
+        <v>3.0999999999999899</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
+      <c r="B53">
+        <v>81.355932203389997</v>
+      </c>
+      <c r="C53">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
+      <c r="B54">
+        <v>82.0512820512822</v>
+      </c>
+      <c r="C54">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
+      <c r="B55">
+        <v>81.355932203389997</v>
+      </c>
+      <c r="C55">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
+      <c r="B56">
+        <v>82.758620689655402</v>
+      </c>
+      <c r="C56">
+        <v>3.2666666666666502</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
+      <c r="B57">
+        <v>82.0512820512822</v>
+      </c>
+      <c r="C57">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
+      <c r="B58">
+        <v>82.758620689655402</v>
+      </c>
+      <c r="C58">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
+      <c r="B59">
+        <v>79.75</v>
+      </c>
+      <c r="C59">
+        <v>3.3333333333333202</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
+      <c r="B60">
+        <v>82.758620689655402</v>
+      </c>
+      <c r="C60">
+        <v>3.0999999999999899</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
+      <c r="B61">
+        <v>85.714285714285893</v>
+      </c>
+      <c r="C61">
+        <v>3.06666666666665</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
+      <c r="B62">
+        <v>85.714285714285893</v>
+      </c>
+      <c r="C62">
+        <v>2.9999999999999898</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
+      <c r="B63">
+        <v>82.758620689655402</v>
+      </c>
+      <c r="C63">
+        <v>3.2666666666666502</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
+      <c r="B64">
+        <v>79.75</v>
+      </c>
+      <c r="C64">
+        <v>3.2333333333333201</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
+      <c r="B65">
+        <v>81.355932203389997</v>
+      </c>
+      <c r="C65">
+        <v>3.2333333333333201</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
+      <c r="B66">
+        <v>82.0512820512822</v>
+      </c>
+      <c r="C66">
+        <v>3.2333333333333201</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
         <f t="shared" ref="A67:A100" si="1">ROW(A66)</f>
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
+      <c r="B67">
+        <v>79.75</v>
+      </c>
+      <c r="C67">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
+      <c r="B68">
+        <v>81.355932203389997</v>
+      </c>
+      <c r="C68">
+        <v>3.2333333333333201</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
+      <c r="B69">
+        <v>83.478260869565403</v>
+      </c>
+      <c r="C69">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="2">
+      <c r="B70">
+        <v>82.758620689655402</v>
+      </c>
+      <c r="C70">
+        <v>3.13333333333332</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="2">
+      <c r="B71">
+        <v>84.210526315789707</v>
+      </c>
+      <c r="C71">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="2">
+      <c r="B72">
+        <v>83.478260869565403</v>
+      </c>
+      <c r="C72">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="2">
+      <c r="B73">
+        <v>82.758620689655402</v>
+      </c>
+      <c r="C73">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="2">
+      <c r="B74">
+        <v>84.210526315789707</v>
+      </c>
+      <c r="C74">
+        <v>3.06666666666665</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="2">
+      <c r="B75">
+        <v>84.955752212389598</v>
+      </c>
+      <c r="C75">
+        <v>3.06666666666665</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
+      <c r="B76">
+        <v>83.478260869565403</v>
+      </c>
+      <c r="C76">
+        <v>3.13333333333332</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="2">
+      <c r="B77">
+        <v>83.478260869565403</v>
+      </c>
+      <c r="C77">
+        <v>3.2333333333333201</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="2">
+      <c r="B78">
+        <v>81.355932203389997</v>
+      </c>
+      <c r="C78">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
+      <c r="B79">
+        <v>79.75</v>
+      </c>
+      <c r="C79">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
+      <c r="B80">
+        <v>82.0512820512822</v>
+      </c>
+      <c r="C80">
+        <v>3.2333333333333201</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
+      <c r="B81">
+        <v>79.75</v>
+      </c>
+      <c r="C81">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="2">
+      <c r="B82">
+        <v>84.210526315789707</v>
+      </c>
+      <c r="C82">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
+      <c r="B83">
+        <v>83.478260869565403</v>
+      </c>
+      <c r="C83">
+        <v>3.06666666666665</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="2">
+      <c r="B84">
+        <v>85.714285714285893</v>
+      </c>
+      <c r="C84">
+        <v>3.13333333333332</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="2">
+      <c r="B85">
+        <v>80.000000000000199</v>
+      </c>
+      <c r="C85">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
+      <c r="B86">
+        <v>86.486486486486697</v>
+      </c>
+      <c r="C86">
+        <v>3.0333333333333199</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="2">
+      <c r="B87">
+        <v>84.210526315789707</v>
+      </c>
+      <c r="C87">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="2">
+      <c r="B88">
+        <v>82.0512820512822</v>
+      </c>
+      <c r="C88">
+        <v>3.13333333333332</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
+      <c r="B89">
+        <v>84.210526315789707</v>
+      </c>
+      <c r="C89">
+        <v>3.13333333333332</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="2">
+      <c r="B90">
+        <v>83.478260869565403</v>
+      </c>
+      <c r="C90">
+        <v>3.13333333333332</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
+      <c r="B91">
+        <v>80.672268907563193</v>
+      </c>
+      <c r="C91">
+        <v>3.2666666666666502</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="2">
+      <c r="B92">
+        <v>84.210526315789707</v>
+      </c>
+      <c r="C92">
+        <v>3.13333333333332</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="2">
+      <c r="B93">
+        <v>82.758620689655402</v>
+      </c>
+      <c r="C93">
+        <v>3.0999999999999899</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="2">
+      <c r="B94">
+        <v>84.210526315789707</v>
+      </c>
+      <c r="C94">
+        <v>3.0999999999999899</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="2">
+      <c r="B95">
+        <v>82.0512820512822</v>
+      </c>
+      <c r="C95">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="2">
+      <c r="B96">
+        <v>83.478260869565403</v>
+      </c>
+      <c r="C96">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="2">
+      <c r="B97">
+        <v>82.0512820512822</v>
+      </c>
+      <c r="C97">
+        <v>3.19999999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="2">
+      <c r="B98">
+        <v>80.672268907563193</v>
+      </c>
+      <c r="C98">
+        <v>3.2666666666666502</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="2">
+      <c r="B99">
+        <v>82.0512820512822</v>
+      </c>
+      <c r="C99">
+        <v>3.2666666666666502</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100">
         <f t="shared" si="1"/>
         <v>99</v>
+      </c>
+      <c r="B100">
+        <v>83.478260869565403</v>
+      </c>
+      <c r="C100">
+        <v>3.1666666666666501</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <v>82.758620689655402</v>
+      </c>
+      <c r="C101">
+        <v>3.1666666666666501</v>
       </c>
     </row>
   </sheetData>

</xml_diff>